<commit_message>
lee factura en imagen con opencv y pytesseract, hace consultas por todo un año dependiendo del restaurante y por mes, año del restaurante. Muestra los resultados de la consulta en un exel
</commit_message>
<xml_diff>
--- a/excel/resultado_consulta.xlsx
+++ b/excel/resultado_consulta.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>#</t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t>Total a pagar</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>2020-07-12</t>
+  </si>
+  <si>
+    <t>2020-01-25</t>
+  </si>
+  <si>
+    <t>2020-01-13</t>
+  </si>
+  <si>
+    <t>2020-08-30</t>
   </si>
 </sst>
 </file>
@@ -366,13 +381,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,36 +409,42 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>123</v>
+        <v>234</v>
       </c>
       <c r="D2">
-        <v>322</v>
+        <v>432</v>
       </c>
       <c r="E2">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="F2">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="G2">
-        <v>93000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>123000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>492</v>
@@ -438,15 +459,18 @@
         <v>7</v>
       </c>
       <c r="G3">
-        <v>43500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>165200</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>492</v>
@@ -463,13 +487,16 @@
       <c r="G4">
         <v>43500</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>492</v>
@@ -485,6 +512,139 @@
       </c>
       <c r="G5">
         <v>43500</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>492</v>
+      </c>
+      <c r="D6">
+        <v>485</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>43500</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>492</v>
+      </c>
+      <c r="D7">
+        <v>485</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>43500</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>492</v>
+      </c>
+      <c r="D8">
+        <v>485</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>43500</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>492</v>
+      </c>
+      <c r="D9">
+        <v>485</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>43500</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>492</v>
+      </c>
+      <c r="D10">
+        <v>485</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>43500</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>